<commit_message>
Changed forecast concept and implemented the required changes
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF64A6C2-A638-411D-A60C-79CA32E2EAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BAB63-1CC1-408B-B070-9AB5C0B1E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>unit</t>
   </si>
@@ -239,9 +239,6 @@
     <t>forecast_data_path</t>
   </si>
   <si>
-    <t>actual_data_path</t>
-  </si>
-  <si>
     <t>file name of forecast data</t>
   </si>
   <si>
@@ -275,18 +272,12 @@
     <t>start time used for parallel processing</t>
   </si>
   <si>
-    <t>not implemented</t>
-  </si>
-  <si>
     <t>QLD</t>
   </si>
   <si>
     <t>01/01/2025</t>
   </si>
   <si>
-    <t>historical_AEMO_Qld1_forecast&amp;settlement_difference_df.csv</t>
-  </si>
-  <si>
     <t>OX2_SunshineState_Old_profile_v1_0.csv</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Price_NSW_Q3_Low.csv</t>
   </si>
   <si>
-    <t>03/01/2025</t>
-  </si>
-  <si>
     <t>SUNSSF_40MW_4hr_results</t>
   </si>
   <si>
@@ -309,6 +297,27 @@
   </si>
   <si>
     <t>TRUE [ FALSE] for multi-threat [single-core] run of the scenario</t>
+  </si>
+  <si>
+    <t>03/10/2025</t>
+  </si>
+  <si>
+    <t>NSW1_dispatch_results.csv</t>
+  </si>
+  <si>
+    <t>forecast_Company</t>
+  </si>
+  <si>
+    <t>The company name that provides the forecast</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Aurora or Baringa</t>
+  </si>
+  <si>
+    <t>Price forecast file</t>
   </si>
 </sst>
 </file>
@@ -342,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,12 +361,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +376,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -384,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,9 +396,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -407,45 +407,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 165 4 2" xfId="1" xr:uid="{0364D493-4BD5-42D4-B16A-2FF2E5465B0E}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -456,6 +487,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}" name="Table5" displayName="Table5" ref="A1:D37" totalsRowShown="0">
+  <autoFilter ref="A1:D37" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B93F956E-F4CA-4E10-9A05-40003B4ABFE8}" name="identifier" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C9D77445-8918-4F42-83C2-E8EFF7212027}" name="description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B45D1B45-C011-456F-8D73-4FE3488C53CF}" name="unit" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{CF3EF38A-5E2C-4BC6-97D0-1A776E1D0AF6}" name="value" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -755,23 +799,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF8ADB6-9146-4145-B9FF-74797635B18C}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -783,40 +827,40 @@
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="13"/>
+      <c r="A3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="9"/>
       <c r="D3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="3">
@@ -824,13 +868,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="3">
@@ -838,13 +882,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="3">
@@ -852,13 +896,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3">
@@ -866,13 +910,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="3">
@@ -880,13 +924,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="3">
@@ -894,13 +938,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3">
@@ -908,13 +952,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3">
@@ -922,13 +966,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3">
@@ -936,13 +980,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3">
@@ -950,13 +994,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3">
@@ -964,93 +1008,89 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5" t="s">
-        <v>81</v>
+      <c r="C19" s="11"/>
+      <c r="D19" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>86</v>
+      <c r="C20" s="11"/>
+      <c r="D20" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="3">
@@ -1058,13 +1098,13 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3">
@@ -1072,13 +1112,13 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="3">
@@ -1086,25 +1126,25 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="3">
@@ -1112,13 +1152,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="A26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="3">
@@ -1126,13 +1166,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="A27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="3">
@@ -1140,13 +1180,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="3">
@@ -1154,13 +1194,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="3">
@@ -1168,25 +1208,25 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="3">
@@ -1194,28 +1234,28 @@
         <v>45657.7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="17">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="3">
@@ -1223,44 +1263,67 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="6" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3" t="s">
-        <v>85</v>
-      </c>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changing the forecast and actual prices
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BAB63-1CC1-408B-B070-9AB5C0B1E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204207A2-B8EE-42D2-B302-664CB66F68D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
   <si>
     <t>unit</t>
   </si>
@@ -275,9 +275,6 @@
     <t>QLD</t>
   </si>
   <si>
-    <t>01/01/2025</t>
-  </si>
-  <si>
     <t>OX2_SunshineState_Old_profile_v1_0.csv</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>TRUE [ FALSE] for multi-threat [single-core] run of the scenario</t>
   </si>
   <si>
-    <t>03/10/2025</t>
-  </si>
-  <si>
     <t>NSW1_dispatch_results.csv</t>
   </si>
   <si>
@@ -318,15 +312,27 @@
   </si>
   <si>
     <t>Price forecast file</t>
+  </si>
+  <si>
+    <t>foresight_period</t>
+  </si>
+  <si>
+    <t>Dispatch period</t>
+  </si>
+  <si>
+    <t>Foresight period to get price forecast and run optimisation</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
+  </si>
+  <si>
+    <t>01/03/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,6 +419,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -422,24 +446,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,15 +453,15 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -490,13 +496,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}" name="Table5" displayName="Table5" ref="A1:D37" totalsRowShown="0">
-  <autoFilter ref="A1:D37" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}" name="Table5" displayName="Table5" ref="A1:D38" totalsRowShown="0">
+  <autoFilter ref="A1:D38" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B93F956E-F4CA-4E10-9A05-40003B4ABFE8}" name="identifier" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{C9D77445-8918-4F42-83C2-E8EFF7212027}" name="description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B45D1B45-C011-456F-8D73-4FE3488C53CF}" name="unit" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{CF3EF38A-5E2C-4BC6-97D0-1A776E1D0AF6}" name="value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B45D1B45-C011-456F-8D73-4FE3488C53CF}" name="unit" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{CF3EF38A-5E2C-4BC6-97D0-1A776E1D0AF6}" name="value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -799,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF8ADB6-9146-4145-B9FF-74797635B18C}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,21 +837,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="3" t="b">
@@ -860,7 +866,7 @@
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="3">
@@ -874,7 +880,7 @@
       <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="3">
@@ -888,7 +894,7 @@
       <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="3">
@@ -902,7 +908,7 @@
       <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3">
@@ -916,7 +922,7 @@
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="3">
@@ -930,7 +936,7 @@
       <c r="B9" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="3">
@@ -944,7 +950,7 @@
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3">
@@ -958,7 +964,7 @@
       <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3">
@@ -972,7 +978,7 @@
       <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3">
@@ -986,7 +992,7 @@
       <c r="B13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3">
@@ -1000,7 +1006,7 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3">
@@ -1014,7 +1020,6 @@
       <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11"/>
       <c r="D15" s="3" t="s">
         <v>78</v>
       </c>
@@ -1026,11 +1031,11 @@
       <c r="B16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1040,23 +1045,22 @@
       <c r="B17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16" t="s">
-        <v>79</v>
+      <c r="D18" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,9 +1070,8 @@
       <c r="B19" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="11"/>
       <c r="D19" s="4" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,9 +1081,8 @@
       <c r="B20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="11"/>
       <c r="D20" s="4" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,7 +1092,7 @@
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="3">
@@ -1104,7 +1106,7 @@
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3">
@@ -1118,7 +1120,7 @@
       <c r="B23" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="3">
@@ -1132,7 +1134,6 @@
       <c r="B24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="11"/>
       <c r="D24" s="3">
         <v>1</v>
       </c>
@@ -1144,7 +1145,7 @@
       <c r="B25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="3">
@@ -1158,7 +1159,7 @@
       <c r="B26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="3">
@@ -1172,7 +1173,7 @@
       <c r="B27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="3">
@@ -1186,7 +1187,7 @@
       <c r="B28" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="3">
@@ -1200,7 +1201,7 @@
       <c r="B29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="3">
@@ -1214,7 +1215,6 @@
       <c r="B30" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="11"/>
       <c r="D30" s="3" t="s">
         <v>40</v>
       </c>
@@ -1226,25 +1226,25 @@
       <c r="B31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="3">
         <f>Inputs!D18-Inputs!D21</f>
-        <v>45657.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+        <v>44926.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="14">
         <v>30</v>
       </c>
     </row>
@@ -1255,68 +1255,79 @@
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="17">
         <v>48</v>
       </c>
-      <c r="B34" s="10" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="C37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="3" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="D38" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1328,33 +1339,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004355FDF4979CB7418AD8D2932A1EEEC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="726943f031c024787d986d883b0a78e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xmlns:ns3="13958d43-bdca-4285-ada7-a2e56a088fb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01cc32bf9c5ce0666932180a5f58ee9a" ns2:_="" ns3:_="">
     <xsd:import namespace="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
@@ -1583,28 +1567,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A2D404-4067-4DC4-A4C2-D764B01DB1E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e3e68ebe-9ec3-4a44-994d-db1f07a01e03"/>
-    <ds:schemaRef ds:uri="4beba541-7443-47a3-924a-216e386cd9c0"/>
-    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
-    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1621,4 +1611,25 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A2D404-4067-4DC4-A4C2-D764B01DB1E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e3e68ebe-9ec3-4a44-994d-db1f07a01e03"/>
+    <ds:schemaRef ds:uri="4beba541-7443-47a3-924a-216e386cd9c0"/>
+    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
+    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes Scenario manager to run several cases
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A55A8A-D920-4B73-9C48-710C0E6BCCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17348B80-541A-4FA5-8CB3-518743CBAF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="SUNSSF" sheetId="3" r:id="rId1"/>
+    <sheet name="ScenarioManager" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
   <si>
     <t>unit</t>
   </si>
@@ -47,9 +48,6 @@
     <t>plant_max_MW</t>
   </si>
   <si>
-    <t>identifier</t>
-  </si>
-  <si>
     <t>Maximum total plant output in MW</t>
   </si>
   <si>
@@ -191,9 +189,6 @@
     <t>This can point towards pre-programmed target functions (representing PPA arrangements etc.)</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>max_FCAS_percent</t>
   </si>
   <si>
@@ -284,9 +279,6 @@
     <t>Price_NSW_Q3_Low.csv</t>
   </si>
   <si>
-    <t>SUNSSF_40MW_4hr_results</t>
-  </si>
-  <si>
     <t>Scenario Name</t>
   </si>
   <si>
@@ -333,13 +325,52 @@
   </si>
   <si>
     <t>2/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The output folder name will include this value </t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Project Sheet</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Scenarios list</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>S1_SUNSSF_40MW_4hr</t>
+  </si>
+  <si>
+    <t>S2_SUNSSF_40MW_4hr</t>
+  </si>
+  <si>
+    <t>S3_SUNSSF_40MW_4hr</t>
+  </si>
+  <si>
+    <t>SUNSSF</t>
+  </si>
+  <si>
+    <t>1,  3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +393,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -377,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -403,6 +448,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -424,9 +493,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,15 +521,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 165 4 2" xfId="1" xr:uid="{0364D493-4BD5-42D4-B16A-2FF2E5465B0E}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -508,13 +583,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}" name="Table5" displayName="Table5" ref="A1:D39" totalsRowShown="0">
-  <autoFilter ref="A1:D39" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B93F956E-F4CA-4E10-9A05-40003B4ABFE8}" name="identifier" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C9D77445-8918-4F42-83C2-E8EFF7212027}" name="description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B45D1B45-C011-456F-8D73-4FE3488C53CF}" name="unit" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CF3EF38A-5E2C-4BC6-97D0-1A776E1D0AF6}" name="value" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FF2B88F-6EF9-4BFC-AD0A-4B173CDF632C}" name="Table52" displayName="Table52" ref="A1:F39" totalsRowShown="0">
+  <autoFilter ref="A1:F39" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{693142CE-3BC7-4F68-BA75-AE3662F66659}" name="Parameter" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DF9BB050-6934-4CD9-8477-35037D2B909B}" name="description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D8257B93-757A-4EB9-B826-85F911E4803F}" name="unit" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7A77A5DA-E91E-4B7B-AB81-893C7A60E45B}" name="1" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{EBA187DC-9709-4F3D-B854-DAE224845ECE}" name="2" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{0E0A6C14-B4D6-4AE3-9166-A69F575269DB}" name="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,11 +893,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF8ADB6-9146-4145-B9FF-74797635B18C}">
-  <dimension ref="A1:E40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68928E6-6D5B-4EA6-9F41-0B06E3209C9D}">
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,13 +905,13 @@
     <col min="1" max="1" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="6" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>3</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -843,524 +920,803 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>4</v>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>14</v>
+      <c r="E3" s="3">
+        <v>128</v>
+      </c>
+      <c r="F3" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3">
         <v>-40</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>13</v>
+      <c r="E4" s="3">
+        <v>-7</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>18</v>
+      <c r="E5" s="3">
+        <v>128</v>
+      </c>
+      <c r="F5" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>19</v>
+      <c r="E6" s="3">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <v>-40</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>63</v>
+      <c r="E7" s="3">
+        <v>-40</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>160</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
+      <c r="E8" s="3">
+        <v>160</v>
+      </c>
+      <c r="F8" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="E9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D10" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
+      <c r="E10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>59</v>
+      <c r="E11" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3">
         <v>0.95189999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>62</v>
+      <c r="E12" s="3">
+        <v>0.95189999999999997</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.95189999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="3">
         <v>0.97160000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="E13" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="E16" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="B19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>34</v>
+      <c r="E20" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>65</v>
+      <c r="E21" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>57</v>
+      <c r="E22" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>30</v>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="E24" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="3">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>58</v>
+      <c r="E26" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="E27" s="3">
+        <v>100</v>
+      </c>
+      <c r="F27" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D28" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="E28" s="3">
+        <v>80</v>
+      </c>
+      <c r="F28" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="E29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="B30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="3">
+        <f>SUNSSF!D17-SUNSSF!D20</f>
+        <v>44926.7</v>
+      </c>
+      <c r="E30" s="3">
+        <f>SUNSSF!E17-SUNSSF!E20</f>
+        <v>44926.7</v>
+      </c>
+      <c r="F30" s="3">
+        <f>SUNSSF!F17-SUNSSF!F20</f>
+        <v>44926.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="3">
-        <f>Inputs!D17-Inputs!D20</f>
-        <v>44926.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D32" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="E32" s="3">
+        <v>30</v>
+      </c>
+      <c r="F32" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>94</v>
+      <c r="E33" s="3">
+        <v>300</v>
+      </c>
+      <c r="F33" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D34" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>97</v>
+      <c r="E34" s="3">
+        <v>48</v>
+      </c>
+      <c r="F34" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D35" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="E35" s="3">
         <v>48</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>50</v>
+      <c r="F35" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
+        <v>79</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72E1691-F2C0-47BF-B23E-0E1DD60C541D}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed Scenario list, removed the last additional day
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17348B80-541A-4FA5-8CB3-518743CBAF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF628A-DFE0-4024-9618-B0D13A13645E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
   <sheets>
     <sheet name="SUNSSF" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="114">
   <si>
     <t>unit</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Scenarios list</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -363,7 +360,25 @@
     <t>SUNSSF</t>
   </si>
   <si>
-    <t>1,  3</t>
+    <t>20/02/2023</t>
+  </si>
+  <si>
+    <t>Explanations/ Example</t>
+  </si>
+  <si>
+    <t>To run simulation</t>
+  </si>
+  <si>
+    <t>TRUE [ FALSE] for including [excluding] scenario from simulation list</t>
+  </si>
+  <si>
+    <t>The sheet name of  selected project</t>
+  </si>
+  <si>
+    <t>21/02/2023</t>
+  </si>
+  <si>
+    <t>20/01/2023</t>
   </si>
 </sst>
 </file>
@@ -477,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,11 +536,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -583,8 +604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FF2B88F-6EF9-4BFC-AD0A-4B173CDF632C}" name="Table52" displayName="Table52" ref="A1:F39" totalsRowShown="0">
-  <autoFilter ref="A1:F39" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FF2B88F-6EF9-4BFC-AD0A-4B173CDF632C}" name="Table52" displayName="Table52" ref="A1:F40" totalsRowShown="0">
+  <autoFilter ref="A1:F40" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{693142CE-3BC7-4F68-BA75-AE3662F66659}" name="Parameter" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{DF9BB050-6934-4CD9-8477-35037D2B909B}" name="description" dataDxfId="4"/>
@@ -894,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68928E6-6D5B-4EA6-9F41-0B06E3209C9D}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +930,7 @@
     <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
@@ -926,381 +947,379 @@
         <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>106</v>
+      <c r="A2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3">
-        <v>128</v>
-      </c>
-      <c r="E3" s="3">
-        <v>128</v>
-      </c>
-      <c r="F3" s="3">
-        <v>128</v>
+        <v>80</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3">
-        <v>-40</v>
+        <v>128</v>
       </c>
       <c r="E4" s="3">
-        <v>-7</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3">
-        <v>-7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="3">
-        <v>128</v>
+        <v>-40</v>
       </c>
       <c r="E5" s="3">
-        <v>128</v>
+        <v>-7</v>
       </c>
       <c r="F5" s="3">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="3">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="E6" s="3">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="F6" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="3">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3">
         <v>-40</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="3">
         <v>-40</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="3">
         <v>-40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>160</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="3">
         <v>160</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="3">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="E10" s="3">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="F10" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="E11" s="3">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="F11" s="3">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3">
-        <v>0.95189999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="E12" s="3">
-        <v>0.95189999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="F12" s="3">
-        <v>0.95189999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3">
-        <v>0.97160000000000002</v>
+        <v>0.95189999999999997</v>
       </c>
       <c r="E13" s="3">
-        <v>0.97160000000000002</v>
+        <v>0.95189999999999997</v>
       </c>
       <c r="F13" s="3">
-        <v>0.97160000000000002</v>
+        <v>0.95189999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.97160000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="18" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
@@ -1315,267 +1334,267 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3">
         <v>0.05</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E23" s="3">
         <v>0.05</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F23" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D24" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F24" s="3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.15</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="F25" s="3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E27" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F27" s="3">
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D28" s="3">
         <v>100</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E28" s="3">
         <v>100</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F28" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D29" s="3">
         <v>80</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E29" s="3">
         <v>80</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="3">
-        <f>SUNSSF!D17-SUNSSF!D20</f>
+      <c r="D31" s="3">
+        <f>SUNSSF!D18-SUNSSF!D21</f>
         <v>44926.7</v>
       </c>
-      <c r="E30" s="3">
-        <f>SUNSSF!E17-SUNSSF!E20</f>
+      <c r="E31" s="3">
+        <f>SUNSSF!E18-SUNSSF!E21</f>
+        <v>44945.7</v>
+      </c>
+      <c r="F31" s="3">
+        <f>SUNSSF!F18-SUNSSF!F21</f>
         <v>44926.7</v>
       </c>
-      <c r="F30" s="3">
-        <f>SUNSSF!F17-SUNSSF!F20</f>
-        <v>44926.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+    </row>
+    <row r="32" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="13" t="b">
+      <c r="C32" s="11"/>
+      <c r="D32" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="E31" s="13" t="b">
+      <c r="E32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13" t="b">
         <v>0</v>
-      </c>
-      <c r="F31" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="3">
-        <v>30</v>
-      </c>
-      <c r="E32" s="3">
-        <v>30</v>
-      </c>
-      <c r="F32" s="3">
-        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="3">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="E33" s="3">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="F33" s="3">
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="3">
+        <v>300</v>
+      </c>
+      <c r="E34" s="3">
+        <v>300</v>
+      </c>
+      <c r="F34" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="3">
-        <v>48</v>
-      </c>
-      <c r="E34" s="3">
-        <v>48</v>
-      </c>
-      <c r="F34" s="3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>90</v>
@@ -1590,82 +1609,102 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="3">
+        <v>48</v>
+      </c>
+      <c r="E36" s="3">
+        <v>48</v>
+      </c>
+      <c r="F36" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B38" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1679,40 +1718,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72E1691-F2C0-47BF-B23E-0E1DD60C541D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>108</v>
+      <c r="B2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1721,6 +1759,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004355FDF4979CB7418AD8D2932A1EEEC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="726943f031c024787d986d883b0a78e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xmlns:ns3="13958d43-bdca-4285-ada7-a2e56a088fb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01cc32bf9c5ce0666932180a5f58ee9a" ns2:_="" ns3:_="">
     <xsd:import namespace="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
@@ -1949,48 +2014,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
-    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2009,9 +2036,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
+    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Export full result datafram
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF628A-DFE0-4024-9618-B0D13A13645E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055816F-CBBB-4354-A632-9D68B5C510DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
@@ -375,10 +375,10 @@
     <t>The sheet name of  selected project</t>
   </si>
   <si>
-    <t>21/02/2023</t>
-  </si>
-  <si>
-    <t>20/01/2023</t>
+    <t>29/01/2023</t>
+  </si>
+  <si>
+    <t>02/02/2023</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,12 +540,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -918,7 +912,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,13 +945,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="18"/>
       <c r="D2" s="3" t="b">
         <v>0</v>
       </c>
@@ -1274,7 +1267,7 @@
         <v>92</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>92</v>
@@ -1291,7 +1284,7 @@
         <v>92</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>92</v>
@@ -1308,7 +1301,7 @@
         <v>107</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>95</v>
@@ -1524,7 +1517,7 @@
       </c>
       <c r="E31" s="3">
         <f>SUNSSF!E18-SUNSSF!E21</f>
-        <v>44945.7</v>
+        <v>44954.7</v>
       </c>
       <c r="F31" s="3">
         <f>SUNSSF!F18-SUNSSF!F21</f>
@@ -1759,33 +1752,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004355FDF4979CB7418AD8D2932A1EEEC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="726943f031c024787d986d883b0a78e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xmlns:ns3="13958d43-bdca-4285-ada7-a2e56a088fb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01cc32bf9c5ce0666932180a5f58ee9a" ns2:_="" ns3:_="">
     <xsd:import namespace="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
@@ -2014,10 +1980,48 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
+    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2036,20 +2040,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
-    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Notations, remove backup excel files
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60234944-5349-4B8E-866E-65F6FCDBC0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DF2C85-DB42-42C1-A54E-FB1CBD93C0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68928E6-6D5B-4EA6-9F41-0B06E3209C9D}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="b">
         <v>0</v>
-      </c>
-      <c r="F2" s="3" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started working on optimisation algorithm
</commit_message>
<xml_diff>
--- a/Input/Project information.xlsx
+++ b/Input/Project information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\341510moja\Documents\GitHub\BESS-V02\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DF2C85-DB42-42C1-A54E-FB1CBD93C0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1243AA-D3AB-48AC-8FAD-8ED12EF289A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B1C603C0-A6AC-4D65-855B-4F102A64A3F9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
   <si>
     <t>unit</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>minutes</t>
-  </si>
-  <si>
-    <t>forecast_res</t>
-  </si>
-  <si>
-    <t>time resolution of the forecast data to be assumed in the solver</t>
   </si>
   <si>
     <t>revenue_method</t>
@@ -601,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FF2B88F-6EF9-4BFC-AD0A-4B173CDF632C}" name="Table52" displayName="Table52" ref="A1:F40" totalsRowShown="0">
-  <autoFilter ref="A1:F40" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FF2B88F-6EF9-4BFC-AD0A-4B173CDF632C}" name="Table52" displayName="Table52" ref="A1:F39" totalsRowShown="0">
+  <autoFilter ref="A1:F39" xr:uid="{47C62E2B-927F-4ECC-8CAE-501F98EC736B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{693142CE-3BC7-4F68-BA75-AE3662F66659}" name="Parameter" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{DF9BB050-6934-4CD9-8477-35037D2B909B}" name="description" dataDxfId="4"/>
@@ -912,15 +906,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68928E6-6D5B-4EA6-9F41-0B06E3209C9D}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -929,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -938,21 +932,21 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="b">
         <v>0</v>
@@ -966,20 +960,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,7 +1081,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
@@ -1164,10 +1158,10 @@
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -1184,10 +1178,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
@@ -1207,16 +1201,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,36 +1221,36 @@
         <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1264,33 +1258,33 @@
         <v>29</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,16 +1292,16 @@
         <v>25</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,10 +1346,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
@@ -1375,7 +1369,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -1389,7 +1383,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>28</v>
@@ -1409,10 +1403,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
@@ -1429,10 +1423,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>9</v>
@@ -1449,10 +1443,10 @@
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>36</v>
@@ -1509,7 +1503,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>23</v>
@@ -1529,10 +1523,10 @@
     </row>
     <row r="32" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="13" t="b">
@@ -1567,33 +1561,33 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="D34" s="3">
-        <v>300</v>
+        <v>48</v>
       </c>
       <c r="E34" s="3">
-        <v>300</v>
+        <v>48</v>
       </c>
       <c r="F34" s="3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3">
         <v>48</v>
@@ -1605,102 +1599,82 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="3">
-        <v>48</v>
-      </c>
-      <c r="E36" s="3">
-        <v>48</v>
-      </c>
-      <c r="F36" s="3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
         <v>46</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="B37" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>81</v>
+      <c r="C38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1729,24 +1703,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1755,6 +1729,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004355FDF4979CB7418AD8D2932A1EEEC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="726943f031c024787d986d883b0a78e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xmlns:ns3="13958d43-bdca-4285-ada7-a2e56a088fb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01cc32bf9c5ce0666932180a5f58ee9a" ns2:_="" ns3:_="">
     <xsd:import namespace="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
@@ -1983,48 +1984,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="13958d43-bdca-4285-ada7-a2e56a088fb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
-    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2043,9 +2006,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA9F891-7B3A-4EF1-87A0-562AC555508D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441C2DA5-EF2A-4B58-9A9A-94482791A20D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78c80c3a-9c8f-4a53-bd4a-4cfbb9f24c43"/>
+    <ds:schemaRef ds:uri="13958d43-bdca-4285-ada7-a2e56a088fb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>